<commit_message>
actualizo archivo raiz del proyecto
</commit_message>
<xml_diff>
--- a/editECU/Plantilla escenarios de caso de uso.xlsx
+++ b/editECU/Plantilla escenarios de caso de uso.xlsx
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -177,15 +177,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -193,25 +199,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,163 +505,159 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B12:D12"/>
@@ -663,6 +668,11 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>